<commit_message>
Minor change to bigdata pipeline
Minor changes to the scripts for the bigdata pipeline + a fix in the studies table (if not paired_end then always overlapping)
</commit_message>
<xml_diff>
--- a/the_real_thing/Excel_files/Studies.xlsx
+++ b/the_real_thing/Excel_files/Studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenio/Dropbox/FMBN/attività17_21/FMBNv4/FMBN4_1_2/FMBN4_1_2_021221/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Dropbox/GitHub_repos/FoodMicrobionet/the_real_thing/Excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A562FB52-22E1-E342-A684-4B246D5C9256}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4466C4C-288F-844C-9FC9-F45DDB273394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="2320" windowWidth="27640" windowHeight="16940" xr2:uid="{74A0AEB2-4F72-6643-A406-D27D786F62F4}"/>
   </bookViews>
@@ -6589,7 +6589,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6937,12 +6937,12 @@
   <dimension ref="A1:AD181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection sqref="A1:AD181"/>
+      <selection activeCell="AC29" sqref="AC29:AC31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7120,13 +7120,13 @@
         <v>54</v>
       </c>
       <c r="AC2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7212,13 +7212,13 @@
         <v>54</v>
       </c>
       <c r="AC3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7304,13 +7304,13 @@
         <v>54</v>
       </c>
       <c r="AC4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7396,13 +7396,13 @@
         <v>54</v>
       </c>
       <c r="AC5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7488,13 +7488,13 @@
         <v>109</v>
       </c>
       <c r="AC6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7580,13 +7580,13 @@
         <v>54</v>
       </c>
       <c r="AC7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7666,13 +7666,13 @@
         <v>54</v>
       </c>
       <c r="AC8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7758,13 +7758,13 @@
         <v>54</v>
       </c>
       <c r="AC9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7850,13 +7850,13 @@
         <v>54</v>
       </c>
       <c r="AC10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7942,13 +7942,13 @@
         <v>54</v>
       </c>
       <c r="AC11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8031,13 +8031,13 @@
         <v>54</v>
       </c>
       <c r="AC12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8123,13 +8123,13 @@
         <v>54</v>
       </c>
       <c r="AC13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8215,13 +8215,13 @@
         <v>54</v>
       </c>
       <c r="AC14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8307,13 +8307,13 @@
         <v>54</v>
       </c>
       <c r="AC15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8393,13 +8393,13 @@
         <v>54</v>
       </c>
       <c r="AC16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8485,13 +8485,13 @@
         <v>54</v>
       </c>
       <c r="AC17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8577,13 +8577,13 @@
         <v>54</v>
       </c>
       <c r="AC18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8666,13 +8666,13 @@
         <v>54</v>
       </c>
       <c r="AC19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8758,13 +8758,13 @@
         <v>54</v>
       </c>
       <c r="AC20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8844,13 +8844,13 @@
         <v>54</v>
       </c>
       <c r="AC21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8936,13 +8936,13 @@
         <v>54</v>
       </c>
       <c r="AC22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9022,13 +9022,13 @@
         <v>54</v>
       </c>
       <c r="AC23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9280,13 +9280,13 @@
         <v>314</v>
       </c>
       <c r="AC26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9363,13 +9363,13 @@
         <v>54</v>
       </c>
       <c r="AC27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9538,13 +9538,13 @@
         <v>347</v>
       </c>
       <c r="AC29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9630,13 +9630,13 @@
         <v>347</v>
       </c>
       <c r="AC30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9722,13 +9722,13 @@
         <v>377</v>
       </c>
       <c r="AC31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9814,7 +9814,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9980,7 +9980,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10238,7 +10238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10662,7 +10662,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10742,7 +10742,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11086,7 +11086,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="49" spans="1:28">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11258,7 +11258,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="50" spans="1:28">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11344,7 +11344,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="51" spans="1:28">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="52" spans="1:28">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="53" spans="1:28">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11602,7 +11602,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="56" spans="1:28">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="57" spans="1:28">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="58" spans="1:28">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="59" spans="1:28">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -12115,7 +12115,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="60" spans="1:28">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="61" spans="1:28">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -12287,7 +12287,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="62" spans="1:28">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="63" spans="1:28">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="64" spans="1:28">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -12545,7 +12545,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="65" spans="1:28">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -12631,7 +12631,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -12717,7 +12717,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="67" spans="1:28">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -12803,7 +12803,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="68" spans="1:28">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -12889,7 +12889,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="69" spans="1:28">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -12975,7 +12975,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="70" spans="1:28">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -13061,7 +13061,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:28">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="72" spans="1:28">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -13233,7 +13233,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="73" spans="1:28">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="74" spans="1:28">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -13405,7 +13405,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="75" spans="1:28">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -13491,7 +13491,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="76" spans="1:28">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="1:28">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="78" spans="1:28">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -13749,7 +13749,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="79" spans="1:28">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -13835,7 +13835,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="80" spans="1:28">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -13921,7 +13921,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="81" spans="1:28">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="82" spans="1:28">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -14093,7 +14093,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="83" spans="1:28">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -14179,7 +14179,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="84" spans="1:28">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -14265,7 +14265,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -14351,7 +14351,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="86" spans="1:28">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="87" spans="1:28">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -14523,7 +14523,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="88" spans="1:28">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -14609,7 +14609,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="89" spans="1:28">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -14695,7 +14695,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="90" spans="1:28">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -14781,7 +14781,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="91" spans="1:28">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="92" spans="1:28">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -14953,7 +14953,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -15039,7 +15039,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="94" spans="1:28">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -15125,7 +15125,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="95" spans="1:28">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -15211,7 +15211,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="96" spans="1:28">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -15297,7 +15297,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="97" spans="1:28">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -15383,7 +15383,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="98" spans="1:28">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -15469,7 +15469,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="99" spans="1:28">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -15555,7 +15555,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="100" spans="1:28">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -15641,7 +15641,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="101" spans="1:28">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -15727,7 +15727,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="102" spans="1:28">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -15813,7 +15813,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="103" spans="1:28">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -15899,7 +15899,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="104" spans="1:28">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -15985,7 +15985,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="105" spans="1:28">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -16068,7 +16068,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="106" spans="1:28">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -16154,7 +16154,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="107" spans="1:28">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -16240,7 +16240,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:28">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -16326,7 +16326,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -16412,7 +16412,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -16498,7 +16498,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="111" spans="1:28">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="112" spans="1:28">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -16670,7 +16670,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="113" spans="1:28">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -16756,7 +16756,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="114" spans="1:28">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16842,7 +16842,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="115" spans="1:28">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16928,7 +16928,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="116" spans="1:28">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -17014,7 +17014,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="117" spans="1:28">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -17100,7 +17100,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="118" spans="1:28">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -17186,7 +17186,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="119" spans="1:28">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -17272,7 +17272,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="120" spans="1:28">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -17358,7 +17358,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="121" spans="1:28">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -17444,7 +17444,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="122" spans="1:28">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -17530,7 +17530,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="123" spans="1:28">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -17616,7 +17616,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="124" spans="1:28">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -17702,7 +17702,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="125" spans="1:28">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -17788,7 +17788,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="126" spans="1:28">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -17874,7 +17874,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="127" spans="1:28">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -17960,7 +17960,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="128" spans="1:28">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -18046,7 +18046,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="129" spans="1:28">
+    <row r="129" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -18132,7 +18132,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="130" spans="1:28">
+    <row r="130" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -18218,7 +18218,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="131" spans="1:28">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -18304,7 +18304,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="132" spans="1:28">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -18384,7 +18384,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="133" spans="1:28">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -18470,7 +18470,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="134" spans="1:28">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -18556,7 +18556,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="135" spans="1:28">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -18642,7 +18642,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="136" spans="1:28">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -18728,7 +18728,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="137" spans="1:28">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -18814,7 +18814,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="138" spans="1:28">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -18900,7 +18900,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="139" spans="1:28">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -18986,7 +18986,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="140" spans="1:28">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -19072,7 +19072,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="141" spans="1:28">
+    <row r="141" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -19158,7 +19158,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="142" spans="1:28">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -19244,7 +19244,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="143" spans="1:28">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -19330,7 +19330,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="144" spans="1:28">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -19416,7 +19416,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="145" spans="1:28">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -19502,7 +19502,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="146" spans="1:28">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -19588,7 +19588,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="147" spans="1:28">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -19674,7 +19674,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="148" spans="1:28">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -19760,7 +19760,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="149" spans="1:28">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -19846,7 +19846,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="150" spans="1:28">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -19932,7 +19932,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="151" spans="1:28">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -20018,7 +20018,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="152" spans="1:28">
+    <row r="152" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -20104,7 +20104,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="153" spans="1:28">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -20190,7 +20190,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="154" spans="1:28">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -20276,7 +20276,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="155" spans="1:28">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -20362,7 +20362,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="156" spans="1:28">
+    <row r="156" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -20448,7 +20448,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="157" spans="1:28">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -20534,7 +20534,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="158" spans="1:28">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -20620,7 +20620,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="159" spans="1:28">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -20706,7 +20706,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="160" spans="1:28">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -20792,7 +20792,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="161" spans="1:30">
+    <row r="161" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -20878,7 +20878,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="162" spans="1:30">
+    <row r="162" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -20964,7 +20964,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="163" spans="1:30">
+    <row r="163" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -21050,7 +21050,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="164" spans="1:30">
+    <row r="164" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -21136,7 +21136,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="165" spans="1:30">
+    <row r="165" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -21222,7 +21222,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="166" spans="1:30">
+    <row r="166" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -21308,7 +21308,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="167" spans="1:30">
+    <row r="167" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="168" spans="1:30">
+    <row r="168" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -21480,7 +21480,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="169" spans="1:30">
+    <row r="169" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -21566,7 +21566,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="170" spans="1:30">
+    <row r="170" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -21652,7 +21652,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="171" spans="1:30">
+    <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -21738,7 +21738,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="172" spans="1:30">
+    <row r="172" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -21830,7 +21830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:30">
+    <row r="173" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -21922,7 +21922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:30">
+    <row r="174" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -22014,7 +22014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:30">
+    <row r="175" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -22106,7 +22106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:30">
+    <row r="176" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -22198,7 +22198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:30">
+    <row r="177" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -22290,7 +22290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:30">
+    <row r="178" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -22382,7 +22382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:30">
+    <row r="179" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -22474,7 +22474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:30">
+    <row r="180" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -22566,7 +22566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:30">
+    <row r="181" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
Changes in the study table
Completed the overlapping and paired_ends columns in study table. Added a comment to readme
</commit_message>
<xml_diff>
--- a/the_real_thing/Excel_files/Studies.xlsx
+++ b/the_real_thing/Excel_files/Studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenioparente/Dropbox/GitHub_repos/FoodMicrobionet/the_real_thing/Excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenio/Dropbox/GitHub_repos/FoodMicrobionet/the_real_thing/Excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4466C4C-288F-844C-9FC9-F45DDB273394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC35EC4-5C6E-6E42-8400-62BDD6C0DB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3700" yWindow="2320" windowWidth="27640" windowHeight="16940" xr2:uid="{74A0AEB2-4F72-6643-A406-D27D786F62F4}"/>
   </bookViews>
@@ -6937,7 +6937,7 @@
   <dimension ref="A1:AD181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29:AC31"/>
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9113,6 +9113,12 @@
       <c r="AB24" t="s">
         <v>293</v>
       </c>
+      <c r="AC24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -9813,8 +9819,14 @@
       <c r="AB32" t="s">
         <v>392</v>
       </c>
+      <c r="AC32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9894,7 +9906,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9980,7 +9992,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10065,8 +10077,14 @@
       <c r="AB35" t="s">
         <v>429</v>
       </c>
+      <c r="AC35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD35" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10151,8 +10169,14 @@
       <c r="AB36" t="s">
         <v>429</v>
       </c>
+      <c r="AC36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD36" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10237,8 +10261,14 @@
       <c r="AB37" t="s">
         <v>54</v>
       </c>
+      <c r="AC37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD37" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10317,8 +10347,14 @@
       <c r="Z38" t="s">
         <v>313</v>
       </c>
+      <c r="AC38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD38" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10403,8 +10439,14 @@
       <c r="AB39" t="s">
         <v>473</v>
       </c>
+      <c r="AC39" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD39" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10489,8 +10531,14 @@
       <c r="AB40" t="s">
         <v>487</v>
       </c>
+      <c r="AC40" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD40" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10575,8 +10623,14 @@
       <c r="AB41" t="s">
         <v>499</v>
       </c>
+      <c r="AC41" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD41" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10661,8 +10715,14 @@
       <c r="AB42" t="s">
         <v>512</v>
       </c>
+      <c r="AC42" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD42" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10741,8 +10801,14 @@
       <c r="Z43" t="s">
         <v>523</v>
       </c>
+      <c r="AC43" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD43" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10827,8 +10893,14 @@
       <c r="AB44" t="s">
         <v>538</v>
       </c>
+      <c r="AC44" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD44" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10913,8 +10985,14 @@
       <c r="AB45" t="s">
         <v>54</v>
       </c>
+      <c r="AC45" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD45" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10999,8 +11077,14 @@
       <c r="AB46" t="s">
         <v>392</v>
       </c>
+      <c r="AC46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD46" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11085,8 +11169,14 @@
       <c r="AB47" t="s">
         <v>473</v>
       </c>
+      <c r="AC47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD47" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11171,8 +11261,14 @@
       <c r="AB48" t="s">
         <v>586</v>
       </c>
+      <c r="AC48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD48" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11257,8 +11353,14 @@
       <c r="AB49" t="s">
         <v>600</v>
       </c>
+      <c r="AC49" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD49" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11343,8 +11445,14 @@
       <c r="AB50" t="s">
         <v>613</v>
       </c>
+      <c r="AC50" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD50" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11429,8 +11537,14 @@
       <c r="AB51" t="s">
         <v>613</v>
       </c>
+      <c r="AC51" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD51" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11515,8 +11629,14 @@
       <c r="AB52" t="s">
         <v>613</v>
       </c>
+      <c r="AC52" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD52" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11601,8 +11721,14 @@
       <c r="AB53" t="s">
         <v>649</v>
       </c>
+      <c r="AC53" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD53" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11687,8 +11813,14 @@
       <c r="AB54" t="s">
         <v>392</v>
       </c>
+      <c r="AC54" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD54" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11773,8 +11905,14 @@
       <c r="AB55" t="s">
         <v>613</v>
       </c>
+      <c r="AC55" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD55" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11859,8 +11997,14 @@
       <c r="AB56" t="s">
         <v>613</v>
       </c>
+      <c r="AC56" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD56" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11945,8 +12089,14 @@
       <c r="AB57" t="s">
         <v>613</v>
       </c>
+      <c r="AC57" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD57" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -12028,8 +12178,14 @@
       <c r="AB58" t="s">
         <v>499</v>
       </c>
+      <c r="AC58" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD58" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -12114,8 +12270,14 @@
       <c r="AB59" t="s">
         <v>717</v>
       </c>
+      <c r="AC59" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD59" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -12200,8 +12362,14 @@
       <c r="AB60" t="s">
         <v>392</v>
       </c>
+      <c r="AC60" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD60" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -12286,8 +12454,14 @@
       <c r="AB61" t="s">
         <v>586</v>
       </c>
+      <c r="AC61" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD61" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -12372,8 +12546,14 @@
       <c r="AB62" t="s">
         <v>613</v>
       </c>
+      <c r="AC62" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD62" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -12458,8 +12638,14 @@
       <c r="AB63" t="s">
         <v>770</v>
       </c>
+      <c r="AC63" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD63" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -12544,8 +12730,14 @@
       <c r="AB64" t="s">
         <v>785</v>
       </c>
+      <c r="AC64" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD64" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -12630,8 +12822,14 @@
       <c r="AB65" t="s">
         <v>586</v>
       </c>
+      <c r="AC65" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD65" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -12716,8 +12914,14 @@
       <c r="AB66" t="s">
         <v>392</v>
       </c>
+      <c r="AC66" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD66" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -12802,8 +13006,14 @@
       <c r="AB67" t="s">
         <v>613</v>
       </c>
+      <c r="AC67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD67" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -12888,8 +13098,14 @@
       <c r="AB68" t="s">
         <v>839</v>
       </c>
+      <c r="AC68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD68" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -12974,8 +13190,14 @@
       <c r="AB69" t="s">
         <v>613</v>
       </c>
+      <c r="AC69" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD69" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -13060,8 +13282,14 @@
       <c r="AB70" t="s">
         <v>54</v>
       </c>
+      <c r="AC70" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD70" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -13146,8 +13374,14 @@
       <c r="AB71" t="s">
         <v>586</v>
       </c>
+      <c r="AC71" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD71" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -13232,8 +13466,14 @@
       <c r="AB72" t="s">
         <v>890</v>
       </c>
+      <c r="AC72" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD72" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -13318,8 +13558,14 @@
       <c r="AB73" t="s">
         <v>586</v>
       </c>
+      <c r="AC73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD73" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -13404,8 +13650,14 @@
       <c r="AB74" t="s">
         <v>347</v>
       </c>
+      <c r="AC74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD74" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -13490,8 +13742,14 @@
       <c r="AB75" t="s">
         <v>347</v>
       </c>
+      <c r="AC75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD75" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -13576,8 +13834,14 @@
       <c r="AB76" t="s">
         <v>586</v>
       </c>
+      <c r="AC76" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD76" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -13662,8 +13926,14 @@
       <c r="AB77" t="s">
         <v>586</v>
       </c>
+      <c r="AC77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD77" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -13748,8 +14018,14 @@
       <c r="AB78" t="s">
         <v>965</v>
       </c>
+      <c r="AC78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD78" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -13834,8 +14110,14 @@
       <c r="AB79" t="s">
         <v>981</v>
       </c>
+      <c r="AC79" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD79" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -13920,8 +14202,14 @@
       <c r="AB80" t="s">
         <v>613</v>
       </c>
+      <c r="AC80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD80" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -14006,8 +14294,14 @@
       <c r="AB81" t="s">
         <v>613</v>
       </c>
+      <c r="AC81" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD81" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -14092,8 +14386,14 @@
       <c r="AB82" t="s">
         <v>586</v>
       </c>
+      <c r="AC82" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD82" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -14178,8 +14478,14 @@
       <c r="AB83" t="s">
         <v>1027</v>
       </c>
+      <c r="AC83" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD83" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -14264,8 +14570,14 @@
       <c r="AB84" t="s">
         <v>392</v>
       </c>
+      <c r="AC84" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD84" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -14350,8 +14662,14 @@
       <c r="AB85" t="s">
         <v>613</v>
       </c>
+      <c r="AC85" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD85" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -14436,8 +14754,14 @@
       <c r="AB86" t="s">
         <v>1066</v>
       </c>
+      <c r="AC86" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD86" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -14522,8 +14846,14 @@
       <c r="AB87" t="s">
         <v>1081</v>
       </c>
+      <c r="AC87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD87" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -14608,8 +14938,14 @@
       <c r="AB88" t="s">
         <v>586</v>
       </c>
+      <c r="AC88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD88" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -14694,8 +15030,14 @@
       <c r="AB89" t="s">
         <v>613</v>
       </c>
+      <c r="AC89" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD89" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -14780,8 +15122,14 @@
       <c r="AB90" t="s">
         <v>1120</v>
       </c>
+      <c r="AC90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD90" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -14866,8 +15214,14 @@
       <c r="AB91" t="s">
         <v>1027</v>
       </c>
+      <c r="AC91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD91" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -14952,8 +15306,14 @@
       <c r="AB92" t="s">
         <v>586</v>
       </c>
+      <c r="AC92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD92" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -15038,8 +15398,14 @@
       <c r="AB93" t="s">
         <v>586</v>
       </c>
+      <c r="AC93" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD93" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -15124,8 +15490,14 @@
       <c r="AB94" t="s">
         <v>586</v>
       </c>
+      <c r="AC94" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD94" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -15210,8 +15582,14 @@
       <c r="AB95" t="s">
         <v>586</v>
       </c>
+      <c r="AC95" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD95" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -15296,8 +15674,14 @@
       <c r="AB96" t="s">
         <v>586</v>
       </c>
+      <c r="AC96" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD96" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -15382,8 +15766,14 @@
       <c r="AB97" t="s">
         <v>1207</v>
       </c>
+      <c r="AC97" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD97" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -15468,8 +15858,14 @@
       <c r="AB98" t="s">
         <v>613</v>
       </c>
+      <c r="AC98" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD98" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -15554,8 +15950,14 @@
       <c r="AB99" t="s">
         <v>1027</v>
       </c>
+      <c r="AC99" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD99" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -15640,8 +16042,14 @@
       <c r="AB100" t="s">
         <v>586</v>
       </c>
+      <c r="AC100" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD100" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -15726,8 +16134,14 @@
       <c r="AB101" t="s">
         <v>613</v>
       </c>
+      <c r="AC101" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD101" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -15812,8 +16226,14 @@
       <c r="AB102" t="s">
         <v>613</v>
       </c>
+      <c r="AC102" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD102" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -15898,8 +16318,14 @@
       <c r="AB103" t="s">
         <v>586</v>
       </c>
+      <c r="AC103" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD103" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -15984,8 +16410,14 @@
       <c r="AB104" t="s">
         <v>586</v>
       </c>
+      <c r="AC104" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD104" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -16067,8 +16499,14 @@
       <c r="AA105" t="s">
         <v>599</v>
       </c>
+      <c r="AC105" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD105" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -16153,8 +16591,14 @@
       <c r="AB106" t="s">
         <v>1317</v>
       </c>
+      <c r="AC106" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD106" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -16239,8 +16683,14 @@
       <c r="AB107" t="s">
         <v>54</v>
       </c>
+      <c r="AC107" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD107" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -16325,8 +16775,14 @@
       <c r="AB108" t="s">
         <v>1339</v>
       </c>
+      <c r="AC108" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD108" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -16411,8 +16867,14 @@
       <c r="AB109" t="s">
         <v>54</v>
       </c>
+      <c r="AC109" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD109" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -16497,8 +16959,14 @@
       <c r="AB110" t="s">
         <v>586</v>
       </c>
+      <c r="AC110" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD110" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -16583,8 +17051,14 @@
       <c r="AB111" t="s">
         <v>586</v>
       </c>
+      <c r="AC111" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD111" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -16669,8 +17143,14 @@
       <c r="AB112" t="s">
         <v>586</v>
       </c>
+      <c r="AC112" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD112" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -16755,8 +17235,14 @@
       <c r="AB113" t="s">
         <v>586</v>
       </c>
+      <c r="AC113" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD113" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -16841,8 +17327,14 @@
       <c r="AB114" t="s">
         <v>586</v>
       </c>
+      <c r="AC114" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD114" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -16927,8 +17419,14 @@
       <c r="AB115" t="s">
         <v>586</v>
       </c>
+      <c r="AC115" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD115" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -17013,8 +17511,14 @@
       <c r="AB116" t="s">
         <v>586</v>
       </c>
+      <c r="AC116" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD116" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -17099,8 +17603,14 @@
       <c r="AB117" t="s">
         <v>586</v>
       </c>
+      <c r="AC117" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD117" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -17185,8 +17695,14 @@
       <c r="AB118" t="s">
         <v>1027</v>
       </c>
+      <c r="AC118" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD118" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -17271,8 +17787,14 @@
       <c r="AB119" t="s">
         <v>613</v>
       </c>
+      <c r="AC119" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD119" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -17357,8 +17879,14 @@
       <c r="AB120" t="s">
         <v>1475</v>
       </c>
+      <c r="AC120" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD120" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -17443,8 +17971,14 @@
       <c r="AB121" t="s">
         <v>586</v>
       </c>
+      <c r="AC121" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD121" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -17529,8 +18063,14 @@
       <c r="AB122" t="s">
         <v>586</v>
       </c>
+      <c r="AC122" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD122" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -17615,8 +18155,14 @@
       <c r="AB123" t="s">
         <v>1513</v>
       </c>
+      <c r="AC123" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD123" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -17701,8 +18247,14 @@
       <c r="AB124" t="s">
         <v>586</v>
       </c>
+      <c r="AC124" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD124" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -17787,8 +18339,14 @@
       <c r="AB125" t="s">
         <v>586</v>
       </c>
+      <c r="AC125" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD125" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -17873,8 +18431,14 @@
       <c r="AB126" t="s">
         <v>1027</v>
       </c>
+      <c r="AC126" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD126" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -17959,8 +18523,14 @@
       <c r="AB127" t="s">
         <v>613</v>
       </c>
+      <c r="AC127" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD127" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -18045,8 +18615,14 @@
       <c r="AB128" t="s">
         <v>1027</v>
       </c>
+      <c r="AC128" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD128" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -18131,8 +18707,14 @@
       <c r="AB129" t="s">
         <v>770</v>
       </c>
+      <c r="AC129" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD129" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -18217,8 +18799,14 @@
       <c r="AB130" t="s">
         <v>1475</v>
       </c>
+      <c r="AC130" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD130" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -18303,8 +18891,14 @@
       <c r="AB131" t="s">
         <v>347</v>
       </c>
+      <c r="AC131" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD131" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -18383,8 +18977,14 @@
       <c r="Z132" t="s">
         <v>375</v>
       </c>
+      <c r="AC132" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD132" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -18469,8 +19069,14 @@
       <c r="AB133" t="s">
         <v>586</v>
       </c>
+      <c r="AC133" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD133" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -18555,8 +19161,14 @@
       <c r="AB134" t="s">
         <v>586</v>
       </c>
+      <c r="AC134" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD134" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -18641,8 +19253,14 @@
       <c r="AB135" t="s">
         <v>586</v>
       </c>
+      <c r="AC135" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD135" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -18727,8 +19345,14 @@
       <c r="AB136" t="s">
         <v>613</v>
       </c>
+      <c r="AC136" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD136" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -18813,8 +19437,14 @@
       <c r="AB137" t="s">
         <v>613</v>
       </c>
+      <c r="AC137" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD137" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -18899,8 +19529,14 @@
       <c r="AB138" t="s">
         <v>586</v>
       </c>
+      <c r="AC138" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD138" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -18985,8 +19621,14 @@
       <c r="AB139" t="s">
         <v>347</v>
       </c>
+      <c r="AC139" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD139" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -19071,8 +19713,14 @@
       <c r="AB140" t="s">
         <v>586</v>
       </c>
+      <c r="AC140" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD140" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -19157,8 +19805,14 @@
       <c r="AB141" t="s">
         <v>586</v>
       </c>
+      <c r="AC141" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD141" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -19243,8 +19897,14 @@
       <c r="AB142" t="s">
         <v>586</v>
       </c>
+      <c r="AC142" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD142" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -19329,8 +19989,14 @@
       <c r="AB143" t="s">
         <v>586</v>
       </c>
+      <c r="AC143" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD143" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -19415,8 +20081,14 @@
       <c r="AB144" t="s">
         <v>586</v>
       </c>
+      <c r="AC144" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD144" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -19501,8 +20173,14 @@
       <c r="AB145" t="s">
         <v>1746</v>
       </c>
+      <c r="AC145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD145" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -19587,8 +20265,14 @@
       <c r="AB146" t="s">
         <v>586</v>
       </c>
+      <c r="AC146" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD146" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -19673,8 +20357,14 @@
       <c r="AB147" t="s">
         <v>586</v>
       </c>
+      <c r="AC147" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD147" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -19759,8 +20449,14 @@
       <c r="AB148" t="s">
         <v>586</v>
       </c>
+      <c r="AC148" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD148" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -19845,8 +20541,14 @@
       <c r="AB149" t="s">
         <v>613</v>
       </c>
+      <c r="AC149" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD149" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -19931,8 +20633,14 @@
       <c r="AB150" t="s">
         <v>586</v>
       </c>
+      <c r="AC150" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD150" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -20017,8 +20725,14 @@
       <c r="AB151" t="s">
         <v>613</v>
       </c>
+      <c r="AC151" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD151" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -20103,8 +20817,14 @@
       <c r="AB152" t="s">
         <v>586</v>
       </c>
+      <c r="AC152" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD152" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -20189,8 +20909,14 @@
       <c r="AB153" t="s">
         <v>1841</v>
       </c>
+      <c r="AC153" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD153" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -20275,8 +21001,14 @@
       <c r="AB154" t="s">
         <v>1856</v>
       </c>
+      <c r="AC154" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD154" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -20361,8 +21093,14 @@
       <c r="AB155" t="s">
         <v>586</v>
       </c>
+      <c r="AC155" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD155" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -20447,8 +21185,14 @@
       <c r="AB156" t="s">
         <v>586</v>
       </c>
+      <c r="AC156" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD156" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -20533,8 +21277,14 @@
       <c r="AB157" t="s">
         <v>473</v>
       </c>
+      <c r="AC157" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD157" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -20619,8 +21369,14 @@
       <c r="AB158" t="s">
         <v>586</v>
       </c>
+      <c r="AC158" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD158" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -20705,8 +21461,14 @@
       <c r="AB159" t="s">
         <v>613</v>
       </c>
+      <c r="AC159" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD159" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -20790,6 +21552,12 @@
       </c>
       <c r="AB160" t="s">
         <v>473</v>
+      </c>
+      <c r="AC160" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD160" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:30" x14ac:dyDescent="0.2">
@@ -20877,6 +21645,12 @@
       <c r="AB161" t="s">
         <v>473</v>
       </c>
+      <c r="AC161" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD161" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -20963,6 +21737,12 @@
       <c r="AB162" t="s">
         <v>1952</v>
       </c>
+      <c r="AC162" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD162" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="163" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -21049,6 +21829,12 @@
       <c r="AB163" t="s">
         <v>1966</v>
       </c>
+      <c r="AC163" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD163" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -21135,6 +21921,12 @@
       <c r="AB164" t="s">
         <v>613</v>
       </c>
+      <c r="AC164" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD164" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="165" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A165">
@@ -21221,6 +22013,12 @@
       <c r="AB165" t="s">
         <v>586</v>
       </c>
+      <c r="AC165" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD165" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="166" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -21307,6 +22105,12 @@
       <c r="AB166" t="s">
         <v>586</v>
       </c>
+      <c r="AC166" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD166" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="167" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A167">
@@ -21393,6 +22197,12 @@
       <c r="AB167" t="s">
         <v>586</v>
       </c>
+      <c r="AC167" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD167" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A168">
@@ -21479,6 +22289,12 @@
       <c r="AB168" t="s">
         <v>586</v>
       </c>
+      <c r="AC168" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD168" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A169">
@@ -21565,6 +22381,12 @@
       <c r="AB169" t="s">
         <v>613</v>
       </c>
+      <c r="AC169" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD169" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="170" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A170">
@@ -21651,6 +22473,12 @@
       <c r="AB170" t="s">
         <v>2049</v>
       </c>
+      <c r="AC170" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD170" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A171">
@@ -21736,6 +22564,12 @@
       </c>
       <c r="AB171" t="s">
         <v>2049</v>
+      </c>
+      <c r="AC171" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD171" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:30" x14ac:dyDescent="0.2">

</xml_diff>